<commit_message>
Test: Skill Set in CharacterDataTable
</commit_message>
<xml_diff>
--- a/GameData/GOCharacterTable.xlsx
+++ b/GameData/GOCharacterTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Epic Games\UE_5.3\GuardiansOrders\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD57858-70D6-451F-A691-345B8D9C497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A839D19-512D-4406-8A74-CF0A90D393F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20130" yWindow="7680" windowWidth="17360" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6550" yWindow="5810" windowWidth="19340" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GOCharacterStatTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Rogers</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -147,6 +147,22 @@
   </si>
   <si>
     <t>GOSkill_Bride_UltimateSkill</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillQ</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillW</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1111,128 +1127,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="30.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="21.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="5" width="16.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.08203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="21.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Test: Skill Set in CharacterDataTable"
This reverts commit 77fad469b3297d76680a0216367e081eedd79d5e.
</commit_message>
<xml_diff>
--- a/GameData/GOCharacterTable.xlsx
+++ b/GameData/GOCharacterTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Epic Games\UE_5.3\GuardiansOrders\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A839D19-512D-4406-8A74-CF0A90D393F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD57858-70D6-451F-A691-345B8D9C497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6550" yWindow="5810" windowWidth="19340" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20130" yWindow="7680" windowWidth="17360" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GOCharacterStatTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Rogers</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -147,22 +147,6 @@
   </si>
   <si>
     <t>GOSkill_Bride_UltimateSkill</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillQ</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillW</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillE</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1127,141 +1111,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="5" width="16.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.08203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
-    <col min="8" max="9" width="21.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.75" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="2" width="30.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="21.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>